<commit_message>
NEWSPAPER VENDOR SHEET UPDATED
NEWSPAPER VENDOR SHEET UPDATED
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/MarketingMaster-Nov-2023.xlsx
+++ b/Offline/BusinessManagement/Marketing/MarketingMaster-Nov-2023.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RoadShow" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="113">
   <si>
     <t>Location</t>
   </si>
@@ -342,6 +342,21 @@
   </si>
   <si>
     <t>Rubi Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRASENJIT </t>
+  </si>
+  <si>
+    <t>CONTACT NUMBER</t>
+  </si>
+  <si>
+    <t>GANGADHAR SARKAR</t>
+  </si>
+  <si>
+    <t>GAUTAM PATRA</t>
+  </si>
+  <si>
+    <t>SUNDAY</t>
   </si>
 </sst>
 </file>
@@ -783,7 +798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -1200,10 +1215,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,9 +1229,10 @@
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1238,34 +1254,67 @@
       <c r="G1" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2">
+        <v>2000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2">
+        <v>150</v>
+      </c>
+      <c r="H2">
+        <v>7980181141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4">
+        <v>2000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4">
+        <v>150</v>
+      </c>
+      <c r="H4">
+        <v>9433501891</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1273,25 +1322,40 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8">
+        <v>3000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8">
+        <v>150</v>
+      </c>
+      <c r="H8">
+        <v>7003901402</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -1299,12 +1363,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -1312,12 +1376,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -1325,12 +1389,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
Updated the status of news paper distribution status
Updated the status of news paper distribution status
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/MarketingMaster-Nov-2023.xlsx
+++ b/Offline/BusinessManagement/Marketing/MarketingMaster-Nov-2023.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C52028-C5D2-4A68-B589-D3697667BF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RoadShow" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="121">
   <si>
     <t>Location</t>
   </si>
@@ -357,12 +358,36 @@
   </si>
   <si>
     <t>SUNDAY</t>
+  </si>
+  <si>
+    <t>Garia Bata Shop</t>
+  </si>
+  <si>
+    <t>Distribution Location</t>
+  </si>
+  <si>
+    <t>Sanjeev Paul</t>
+  </si>
+  <si>
+    <t>Call him on 5th December for booking on 10th December</t>
+  </si>
+  <si>
+    <t>Distribution Date</t>
+  </si>
+  <si>
+    <t>Call Sanjeev Paul</t>
+  </si>
+  <si>
+    <t>Getting Switched Off</t>
+  </si>
+  <si>
+    <t>Did not pick up the call</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -387,7 +412,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,6 +422,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -454,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -472,7 +503,6 @@
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,7 +511,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -492,6 +521,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +541,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -550,9 +586,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -587,7 +623,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -622,7 +658,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -795,25 +831,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="82.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="82.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -836,7 +872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -853,7 +889,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -867,7 +903,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -881,7 +917,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -895,7 +931,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -909,7 +945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -923,7 +959,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -937,7 +973,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -951,7 +987,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -965,7 +1001,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -986,39 +1022,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16" width="13.28515625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="5"/>
+    <col min="3" max="3" width="5.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="13.33203125" style="5" customWidth="1"/>
+    <col min="17" max="17" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
@@ -1077,7 +1113,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
@@ -1086,13 +1122,13 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
     </row>
-    <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>40</v>
       </c>
@@ -1100,7 +1136,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>41</v>
       </c>
@@ -1108,7 +1144,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>42</v>
       </c>
@@ -1116,7 +1152,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>43</v>
       </c>
@@ -1124,7 +1160,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>48</v>
       </c>
@@ -1132,7 +1168,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -1140,17 +1176,17 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>47</v>
       </c>
@@ -1162,26 +1198,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>67</v>
       </c>
@@ -1214,235 +1250,307 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="48.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.21875" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>64</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>108</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>2000</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>112</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>150</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>7980181141</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="J2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D4">
+      <c r="E4" s="17">
         <v>2000</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="17"/>
+      <c r="H4" s="17">
         <v>150</v>
       </c>
-      <c r="H4">
+      <c r="I4" s="17">
         <v>9433501891</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="J4" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6">
+        <v>2000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="19">
+        <v>0.1875</v>
+      </c>
+      <c r="I6">
+        <v>9831570813</v>
+      </c>
+      <c r="J6" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" s="18">
+        <v>45270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>55</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>56</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C10" t="s">
         <v>64</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D10" t="s">
         <v>110</v>
       </c>
-      <c r="D8">
+      <c r="E10">
         <v>3000</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F10" t="s">
         <v>112</v>
       </c>
-      <c r="G8">
+      <c r="H10">
         <v>150</v>
       </c>
-      <c r="H8">
+      <c r="I10">
         <v>7003901402</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="J10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>57</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>58</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>59</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>60</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>61</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>62</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>63</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C24" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1452,61 +1560,61 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="13"/>
-      <c r="C2" s="16" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="12"/>
+      <c r="C2" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="17" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="11"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+      <c r="G2" s="16"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="10">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="9">
         <v>1</v>
       </c>
       <c r="C4" t="s">
@@ -1515,7 +1623,7 @@
       <c r="D4" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="13">
         <v>0.2590277777777778</v>
       </c>
       <c r="F4">
@@ -1525,8 +1633,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="10">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="9">
         <v>2</v>
       </c>
       <c r="C5" t="s">
@@ -1535,7 +1643,7 @@
       <c r="D5" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="13">
         <v>0.26041666666666669</v>
       </c>
       <c r="F5">
@@ -1545,8 +1653,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="10">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="9">
         <v>3</v>
       </c>
       <c r="C6" t="s">
@@ -1555,12 +1663,12 @@
       <c r="D6" t="s">
         <v>92</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="13">
         <v>0.2638888888888889</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="10">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="9">
         <v>4</v>
       </c>
       <c r="C7" t="s">
@@ -1569,12 +1677,12 @@
       <c r="D7" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="13">
         <v>0.26527777777777778</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="10">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="9">
         <v>5</v>
       </c>
       <c r="C8" t="s">
@@ -1583,12 +1691,12 @@
       <c r="D8" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="13">
         <v>0.26944444444444443</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="10">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="9">
         <v>6</v>
       </c>
       <c r="C9" t="s">
@@ -1597,12 +1705,12 @@
       <c r="D9" t="s">
         <v>92</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="13">
         <v>0.27361111111111108</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="10">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="9">
         <v>7</v>
       </c>
       <c r="C10" t="s">
@@ -1611,12 +1719,12 @@
       <c r="D10" t="s">
         <v>94</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="13">
         <v>0.27638888888888885</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="10">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="9">
         <v>8</v>
       </c>
       <c r="C11" t="s">
@@ -1625,12 +1733,12 @@
       <c r="D11" t="s">
         <v>95</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="13">
         <v>0.27777777777777779</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="10">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="9">
         <v>9</v>
       </c>
       <c r="C12" t="s">
@@ -1639,12 +1747,12 @@
       <c r="D12" t="s">
         <v>96</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="13">
         <v>0.27847222222222223</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="10">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="9">
         <v>10</v>
       </c>
       <c r="C13" t="s">
@@ -1653,12 +1761,12 @@
       <c r="D13" t="s">
         <v>97</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="13">
         <v>0.27847222222222223</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="10">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="9">
         <v>11</v>
       </c>
       <c r="C14" t="s">
@@ -1667,12 +1775,12 @@
       <c r="D14" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="13">
         <v>0.28125</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="10">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="9">
         <v>12</v>
       </c>
       <c r="C15" t="s">
@@ -1681,7 +1789,7 @@
       <c r="D15" t="s">
         <v>99</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="13">
         <v>0.28472222222222221</v>
       </c>
       <c r="F15">
@@ -1691,8 +1799,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="10">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="9">
         <v>13</v>
       </c>
       <c r="C16" t="s">
@@ -1701,12 +1809,12 @@
       <c r="D16" t="s">
         <v>100</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="13">
         <v>0.28611111111111115</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="10">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="9">
         <v>14</v>
       </c>
       <c r="C17" t="s">
@@ -1715,12 +1823,12 @@
       <c r="D17" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="13">
         <v>0.28680555555555554</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="10">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="9">
         <v>15</v>
       </c>
       <c r="C18" t="s">
@@ -1729,12 +1837,12 @@
       <c r="D18" t="s">
         <v>102</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="13">
         <v>0.28888888888888892</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="10">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="9">
         <v>16</v>
       </c>
       <c r="C19" t="s">
@@ -1743,12 +1851,12 @@
       <c r="D19" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="13">
         <v>0.2902777777777778</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="10">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="9">
         <v>17</v>
       </c>
       <c r="C20" t="s">
@@ -1757,12 +1865,12 @@
       <c r="D20" t="s">
         <v>104</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="13">
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="10">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="9">
         <v>18</v>
       </c>
       <c r="C21" t="s">
@@ -1771,12 +1879,12 @@
       <c r="D21" t="s">
         <v>105</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="13">
         <v>0.29791666666666666</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="10">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="9">
         <v>19</v>
       </c>
       <c r="C22" t="s">
@@ -1785,12 +1893,12 @@
       <c r="D22" t="s">
         <v>106</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="13">
         <v>0.30208333333333331</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="10">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="9">
         <v>20</v>
       </c>
       <c r="C23" t="s">
@@ -1799,12 +1907,12 @@
       <c r="D23" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="13">
         <v>0.30208333333333331</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="10">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="9">
         <v>21</v>
       </c>
       <c r="C24" t="s">
@@ -1813,12 +1921,12 @@
       <c r="D24" t="s">
         <v>107</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="13">
         <v>0.3125</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E26" s="15"/>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E26" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Enquiry work book Updated with 3 sheets
Enquiry Sheet Updated with 3 sheets
a) Prospects
b) Old Prospects
c) Notes
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/MarketingMaster-Nov-2023.xlsx
+++ b/Offline/BusinessManagement/Marketing/MarketingMaster-Nov-2023.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C52028-C5D2-4A68-B589-D3697667BF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123AB642-0629-414A-A933-1C6C423493A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,14 +12,15 @@
     <sheet name="SchoolGate" sheetId="2" r:id="rId2"/>
     <sheet name="FB" sheetId="3" r:id="rId3"/>
     <sheet name="NewsPaper" sheetId="4" r:id="rId4"/>
-    <sheet name="BusRoute" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
+    <sheet name="BusRoute" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="125">
   <si>
     <t>Location</t>
   </si>
@@ -378,10 +379,22 @@
     <t>Call Sanjeev Paul</t>
   </si>
   <si>
-    <t>Getting Switched Off</t>
-  </si>
-  <si>
-    <t>Did not pick up the call</t>
+    <t>Sanjeev Mazumdar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bappa </t>
+  </si>
+  <si>
+    <t>Call him in the evening today on 02-12-2023</t>
+  </si>
+  <si>
+    <t>Did not pick up the call. Sanjeev will inform Prasenjit to call</t>
+  </si>
+  <si>
+    <t>Entrance of Floating Market</t>
+  </si>
+  <si>
+    <t>Note: Connect with Sanjeev Mazumdar @ 9433265655, if any one of the above agent is not available.</t>
   </si>
 </sst>
 </file>
@@ -485,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -512,6 +525,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -521,9 +537,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,10 +555,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1251,16 +1263,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
@@ -1268,7 +1280,7 @@
     <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="48.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="49.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.21875" customWidth="1"/>
     <col min="13" max="13" width="11.6640625" customWidth="1"/>
@@ -1313,6 +1325,9 @@
       <c r="A2" t="s">
         <v>53</v>
       </c>
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
       <c r="C2" t="s">
         <v>64</v>
       </c>
@@ -1325,6 +1340,9 @@
       <c r="F2" t="s">
         <v>112</v>
       </c>
+      <c r="G2" s="13">
+        <v>0.21875</v>
+      </c>
       <c r="H2">
         <v>150</v>
       </c>
@@ -1332,7 +1350,10 @@
         <v>7980181141</v>
       </c>
       <c r="J2" t="s">
-        <v>120</v>
+        <v>122</v>
+      </c>
+      <c r="K2" s="15">
+        <v>45263</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1341,46 +1362,46 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="14">
         <v>2000</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17">
+      <c r="G4" s="14"/>
+      <c r="H4" s="14">
         <v>150</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4" s="14">
         <v>9433501891</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="14" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1401,7 +1422,7 @@
       <c r="F6" t="s">
         <v>112</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="16">
         <v>0.1875</v>
       </c>
       <c r="I6">
@@ -1410,7 +1431,7 @@
       <c r="J6" t="s">
         <v>116</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="15">
         <v>45270</v>
       </c>
     </row>
@@ -1455,7 +1476,7 @@
         <v>7003901402</v>
       </c>
       <c r="J10" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1497,12 +1518,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -1510,12 +1531,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -1523,12 +1544,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -1536,12 +1557,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -1549,9 +1570,51 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A28:E28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C70299E-C0F5-4E3E-8E74-918F4B61E676}">
+  <dimension ref="D2:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2">
+        <v>9433265655</v>
       </c>
     </row>
   </sheetData>
@@ -1559,7 +1622,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:H26"/>
   <sheetViews>
@@ -1579,15 +1642,15 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="12"/>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="16"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="10"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Enquiry work Updated with 2 sheets
Enquiry work Updated with 2 sheets
a) Prospects
b) Notes
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/MarketingMaster-Nov-2023.xlsx
+++ b/Offline/BusinessManagement/Marketing/MarketingMaster-Nov-2023.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123AB642-0629-414A-A933-1C6C423493A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C4F67C-670E-43EC-B5A4-AE4D4F52806F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,15 +12,14 @@
     <sheet name="SchoolGate" sheetId="2" r:id="rId2"/>
     <sheet name="FB" sheetId="3" r:id="rId3"/>
     <sheet name="NewsPaper" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
-    <sheet name="BusRoute" sheetId="5" r:id="rId6"/>
+    <sheet name="BusRoute" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="123">
   <si>
     <t>Location</t>
   </si>
@@ -377,12 +376,6 @@
   </si>
   <si>
     <t>Call Sanjeev Paul</t>
-  </si>
-  <si>
-    <t>Sanjeev Mazumdar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bappa </t>
   </si>
   <si>
     <t>Call him in the evening today on 02-12-2023</t>
@@ -528,6 +521,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -536,9 +532,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1265,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1326,7 +1319,7 @@
         <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
         <v>64</v>
@@ -1350,7 +1343,7 @@
         <v>7980181141</v>
       </c>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K2" s="15">
         <v>45263</v>
@@ -1476,7 +1469,7 @@
         <v>7003901402</v>
       </c>
       <c r="J10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1576,13 +1569,13 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
+      <c r="A28" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1593,36 +1586,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C70299E-C0F5-4E3E-8E74-918F4B61E676}">
-  <dimension ref="D2:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G2">
-        <v>9433265655</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:H26"/>
   <sheetViews>
@@ -1642,15 +1605,15 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="12"/>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="17"/>
+      <c r="D2" s="18"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="19"/>
+      <c r="G2" s="20"/>
       <c r="H2" s="10"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Ops done for Physics and Maths class
Ops done for Physics and Maths class
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/MarketingMaster-Nov-2023.xlsx
+++ b/Offline/BusinessManagement/Marketing/MarketingMaster-Nov-2023.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C4F67C-670E-43EC-B5A4-AE4D4F52806F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C54029-744B-4D8B-9CB4-AAF05B498E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,21 +345,6 @@
     <t>Rubi Park</t>
   </si>
   <si>
-    <t xml:space="preserve">PRASENJIT </t>
-  </si>
-  <si>
-    <t>CONTACT NUMBER</t>
-  </si>
-  <si>
-    <t>GANGADHAR SARKAR</t>
-  </si>
-  <si>
-    <t>GAUTAM PATRA</t>
-  </si>
-  <si>
-    <t>SUNDAY</t>
-  </si>
-  <si>
     <t>Garia Bata Shop</t>
   </si>
   <si>
@@ -388,6 +373,21 @@
   </si>
   <si>
     <t>Note: Connect with Sanjeev Mazumdar @ 9433265655, if any one of the above agent is not available.</t>
+  </si>
+  <si>
+    <t>Prasenjit</t>
+  </si>
+  <si>
+    <t>Gautam Patra</t>
+  </si>
+  <si>
+    <t>Gangadhar Sarkar</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Contact No.</t>
   </si>
 </sst>
 </file>
@@ -1258,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1272,7 +1272,7 @@
     <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="49.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.21875" customWidth="1"/>
@@ -1284,7 +1284,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>49</v>
@@ -1305,13 +1305,13 @@
         <v>66</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1319,19 +1319,19 @@
         <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
         <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="E2">
         <v>2000</v>
       </c>
       <c r="F2" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="G2" s="13">
         <v>0.21875</v>
@@ -1343,7 +1343,7 @@
         <v>7980181141</v>
       </c>
       <c r="J2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="K2" s="15">
         <v>45263</v>
@@ -1363,13 +1363,13 @@
         <v>64</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E4" s="14">
         <v>2000</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="14">
@@ -1379,7 +1379,7 @@
         <v>9433501891</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1401,19 +1401,19 @@
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
         <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E6">
         <v>2000</v>
       </c>
       <c r="F6" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="G6" s="16">
         <v>0.1875</v>
@@ -1422,7 +1422,7 @@
         <v>9831570813</v>
       </c>
       <c r="J6" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="K6" s="15">
         <v>45270</v>
@@ -1454,13 +1454,13 @@
         <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E10">
         <v>3000</v>
       </c>
       <c r="F10" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="H10">
         <v>150</v>
@@ -1469,7 +1469,7 @@
         <v>7003901402</v>
       </c>
       <c r="J10" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1570,7 +1570,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>

</xml_diff>